<commit_message>
start the analyzer code
start the analyzer code
</commit_message>
<xml_diff>
--- a/modera_decatur.xlsx
+++ b/modera_decatur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlp\Documents\GitHub\nus_apartment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9218025-8FDF-4908-887C-1F5F99E19EB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573DCB71-8BDE-4CCA-8B53-A846B851AEA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" firstSheet="3" activeTab="10" xr2:uid="{0613D09A-7280-4844-B453-E571AA672FAC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" firstSheet="2" activeTab="2" xr2:uid="{0613D09A-7280-4844-B453-E571AA672FAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Identification" sheetId="2" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="Expense" sheetId="5" r:id="rId7"/>
     <sheet name="ConstructionLoan" sheetId="6" r:id="rId8"/>
     <sheet name="PermanentLoan" sheetId="7" r:id="rId9"/>
-    <sheet name="Equity" sheetId="8" r:id="rId10"/>
-    <sheet name="CapEx" sheetId="9" r:id="rId11"/>
+    <sheet name="AssetMgmt" sheetId="8" r:id="rId10"/>
+    <sheet name="waterfall" sheetId="13" r:id="rId11"/>
+    <sheet name="CapEx" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
   <si>
     <t>Project Name</t>
   </si>
@@ -247,12 +248,6 @@
     <t>cpi</t>
   </si>
   <si>
-    <t>pfd_return</t>
-  </si>
-  <si>
-    <t>compound</t>
-  </si>
-  <si>
     <t>quarter</t>
   </si>
   <si>
@@ -301,9 +296,6 @@
     <t>Start_date</t>
   </si>
   <si>
-    <t>Shovel_ready_date</t>
-  </si>
-  <si>
     <t>Overhead</t>
   </si>
   <si>
@@ -368,6 +360,18 @@
   </si>
   <si>
     <t>Total_predevelop</t>
+  </si>
+  <si>
+    <t>month_incur</t>
+  </si>
+  <si>
+    <t>stat</t>
+  </si>
+  <si>
+    <t>hurdle</t>
+  </si>
+  <si>
+    <t>Permit_issued</t>
   </si>
 </sst>
 </file>
@@ -376,7 +380,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -420,8 +424,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -740,7 +744,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -767,15 +771,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -783,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -791,7 +795,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -799,15 +803,15 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -852,7 +856,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C13">
         <f>SUM(C11:C12)</f>
@@ -861,7 +865,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D14">
         <v>240</v>
@@ -874,15 +878,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5876C29A-619F-49C0-B706-69A3D1B8DE75}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -890,49 +894,24 @@
         <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B2" s="2">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="2">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -941,10 +920,49 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399DA196-FC76-4565-9BCA-48468CDE8348}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771963C5-A621-408D-B251-D1D58ECD5746}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1136,20 +1154,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EF6FA6-86BA-44C6-930E-9327A33FA58E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="9.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -1159,22 +1179,28 @@
       <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3">
         <v>43678</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1182,44 +1208,44 @@
       <c r="C3" s="4">
         <v>12000000</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4">
         <v>4000000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>25000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6">
-        <f>D4</f>
+        <v>101</v>
+      </c>
+      <c r="E6">
+        <f>E4</f>
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="4">
-        <f>SUM(C3:C4)+D6*E5</f>
+        <v>97</v>
+      </c>
+      <c r="G7" s="4">
+        <f>SUM(C3:C4)+E6*F5</f>
         <v>16300000</v>
       </c>
     </row>
@@ -1230,19 +1256,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03C2508-7A59-43F9-A39B-16656D2BC02C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="4" max="4" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -1258,8 +1284,11 @@
       <c r="E1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1273,7 +1302,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1287,7 +1316,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1302,7 +1331,7 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1317,7 +1346,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1331,33 +1360,33 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E7" s="4">
         <f>3000000/18</f>
         <v>166666.66666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C8" cm="1">
         <f t="array" ref="C8">MAX(B2:B6+C2:C6)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1366,11 +1395,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="4">
+        <v>78</v>
+      </c>
+      <c r="F11" s="4">
         <f>SUM(D2:D7)+C8*E7</f>
         <v>68000000</v>
       </c>
@@ -1413,7 +1442,7 @@
         <v>54</v>
       </c>
       <c r="H1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -1522,7 +1551,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1547,7 +1576,7 @@
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
         <v>54</v>
@@ -1562,12 +1591,12 @@
         <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D2">
         <v>0.37</v>
@@ -1581,13 +1610,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C3">
         <v>250000</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -1595,13 +1624,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4">
         <v>800000</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H4">
         <v>11</v>
@@ -1609,7 +1638,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F5" s="2">
         <v>2.5000000000000001E-2</v>
@@ -1650,7 +1679,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1">
         <v>0.65</v>
@@ -1658,17 +1687,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4">
-        <f>B2*(Construction!D11+Predevelopment!C7)</f>
+        <f>B2*(Construction!F11+Predevelopment!G7)</f>
         <v>54795000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="5">
         <f>D4*C3*CapMarkets!B3</f>
@@ -1680,7 +1709,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" s="5">
         <f>SUM(C3:C4)</f>
@@ -1713,12 +1742,12 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1726,7 +1755,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1">
         <v>0.6</v>
@@ -1734,7 +1763,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1742,7 +1771,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -1750,7 +1779,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2">
         <v>1.4999999999999999E-2</v>

</xml_diff>

<commit_message>
added revenue and expenses
</commit_message>
<xml_diff>
--- a/modera_decatur.xlsx
+++ b/modera_decatur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlp\Documents\GitHub\nus_apartment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807D6EE1-73B5-48A8-BED3-CA07651F1337}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69214D3-FF4F-4643-86C2-A206343C900F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" firstSheet="2" activeTab="3" xr2:uid="{0613D09A-7280-4844-B453-E571AA672FAC}"/>
+    <workbookView xWindow="5625" yWindow="5205" windowWidth="16875" windowHeight="9195" firstSheet="3" activeTab="4" xr2:uid="{0613D09A-7280-4844-B453-E571AA672FAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Identification" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
   <si>
     <t>Project Name</t>
   </si>
@@ -160,9 +160,6 @@
     <t>pct_per_yr</t>
   </si>
   <si>
-    <t>n-month</t>
-  </si>
-  <si>
     <t>Lobby_renew</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>pct_of_rev</t>
   </si>
   <si>
-    <t>pct_of_asset</t>
-  </si>
-  <si>
     <t>increase</t>
   </si>
   <si>
@@ -334,15 +328,9 @@
     <t>property_mgmt</t>
   </si>
   <si>
-    <t>cpi+1</t>
-  </si>
-  <si>
     <t>Total_predevelop</t>
   </si>
   <si>
-    <t>month_incur</t>
-  </si>
-  <si>
     <t>stat</t>
   </si>
   <si>
@@ -353,6 +341,21 @@
   </si>
   <si>
     <t>end_month</t>
+  </si>
+  <si>
+    <t>Cost_overrun</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>expense_sensitivity</t>
+  </si>
+  <si>
+    <t>cpi+.01</t>
+  </si>
+  <si>
+    <t>revenue_sensitivity</t>
   </si>
 </sst>
 </file>
@@ -735,7 +738,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -752,15 +755,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -768,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -776,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -784,15 +787,15 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -837,7 +840,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13">
         <f>SUM(C11:C12)</f>
@@ -846,7 +849,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14">
         <v>240</v>
@@ -869,13 +872,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -883,16 +886,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -905,17 +908,17 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -928,10 +931,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="B3" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -956,30 +959,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1000000</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -990,13 +993,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>2000000</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>7</v>
@@ -1007,14 +1010,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <f>20*Identification!C11</f>
         <v>4632980</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -1025,7 +1028,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>1000000</v>
@@ -1039,7 +1042,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>2000000</v>
@@ -1053,7 +1056,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>500000</v>
@@ -1084,7 +1087,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -1095,7 +1098,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1">
         <v>0.02</v>
@@ -1135,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EF6FA6-86BA-44C6-930E-9327A33FA58E}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1150,9 +1153,9 @@
     <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1161,27 +1164,30 @@
         <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3">
         <v>43678</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1192,19 +1198,25 @@
       <c r="D3" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4">
         <v>4000000</v>
       </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
       <c r="E4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1212,22 +1224,30 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E6">
         <f>E4</f>
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G7" s="4">
         <f>SUM(C3:C4)+E6*F5</f>
         <v>16300000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1237,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03C2508-7A59-43F9-A39B-16656D2BC02C}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1249,27 +1269,33 @@
     <col min="5" max="6" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1283,7 +1309,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1297,7 +1323,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1311,7 +1337,7 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1326,7 +1352,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1340,33 +1366,33 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7" s="4">
         <f>3000000/18</f>
         <v>166666.66666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8">
         <f>MAX(C2:C6)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1375,13 +1401,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F11" s="4">
         <f>SUM(D2:D7)+C8*E7</f>
         <v>68000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1391,23 +1433,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CA4446-BDCA-40AA-A549-CCDDEA333C10}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U28" sqref="U21:U28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>25</v>
@@ -1416,13 +1458,13 @@
         <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -1463,14 +1505,19 @@
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>55000</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1482,15 +1529,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E0346C-7E83-4155-8A21-FD59FFB9DB4B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>37</v>
@@ -1528,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E0963A-52B8-4079-B831-243F6B7AA707}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1541,87 +1586,94 @@
     <col min="4" max="4" width="12.59765625" customWidth="1"/>
     <col min="5" max="5" width="7.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
       <c r="I1" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D2">
         <v>0.37</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3">
         <v>250000</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3">
+        <v>102</v>
+      </c>
+      <c r="G3">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4">
         <v>800000</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4">
+        <v>102</v>
+      </c>
+      <c r="G4">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F5" s="2">
         <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1697,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
@@ -1654,12 +1706,12 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1">
         <v>0.65</v>
@@ -1667,7 +1719,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4">
@@ -1677,7 +1729,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="5">
         <f>D4*C3*CapMarkets!B3</f>
@@ -1689,7 +1741,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="5">
         <f>SUM(C3:C4)</f>
@@ -1713,7 +1765,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -1722,12 +1774,12 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1735,7 +1787,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1">
         <v>0.6</v>
@@ -1743,7 +1795,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1751,7 +1803,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -1759,7 +1811,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2">
         <v>1.4999999999999999E-2</v>

</xml_diff>

<commit_message>
complete unlevered cash flow
</commit_message>
<xml_diff>
--- a/modera_decatur.xlsx
+++ b/modera_decatur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlp\Documents\GitHub\nus_apartment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69214D3-FF4F-4643-86C2-A206343C900F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA74538D-019F-467F-B4B7-FFA9CE3D0FCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="5205" windowWidth="16875" windowHeight="9195" firstSheet="3" activeTab="4" xr2:uid="{0613D09A-7280-4844-B453-E571AA672FAC}"/>
+    <workbookView xWindow="5625" yWindow="5205" windowWidth="16875" windowHeight="9195" firstSheet="6" activeTab="11" xr2:uid="{0613D09A-7280-4844-B453-E571AA672FAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Identification" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="103">
   <si>
     <t>Project Name</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>HVAC</t>
-  </si>
-  <si>
-    <t>Electrical</t>
   </si>
   <si>
     <t>Elevators</t>
@@ -738,7 +735,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -755,15 +752,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
         <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -771,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -779,7 +776,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -787,15 +784,15 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
         <v>83</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -840,7 +837,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13">
         <f>SUM(C11:C12)</f>
@@ -849,7 +846,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D14">
         <v>240</v>
@@ -872,13 +869,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -886,16 +883,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -915,10 +912,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -944,10 +941,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771963C5-A621-408D-B251-D1D58ECD5746}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -959,19 +956,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
         <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -982,7 +979,7 @@
         <v>1000000</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -999,7 +996,7 @@
         <v>2000000</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>7</v>
@@ -1010,14 +1007,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <f>20*Identification!C11</f>
         <v>4632980</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -1033,6 +1030,9 @@
       <c r="B5">
         <v>1000000</v>
       </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
       <c r="D5">
         <v>15</v>
       </c>
@@ -1045,24 +1045,16 @@
         <v>41</v>
       </c>
       <c r="B6">
-        <v>2000000</v>
+        <v>500000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7">
-        <v>500000</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1087,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -1098,7 +1090,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1">
         <v>0.02</v>
@@ -1155,7 +1147,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1167,13 +1159,13 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -1181,7 +1173,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3">
         <v>43678</v>
@@ -1226,7 +1218,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6">
         <f>E4</f>
@@ -1235,7 +1227,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="4">
         <f>SUM(C3:C4)+E6*F5</f>
@@ -1244,7 +1236,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1271,22 +1263,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
         <v>24</v>
@@ -1368,7 +1360,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="4">
         <f>3000000/18</f>
@@ -1377,7 +1369,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8">
         <f>MAX(C2:C6)</f>
@@ -1386,7 +1378,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1403,7 +1395,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="4">
         <f>SUM(D2:D7)+C8*E7</f>
@@ -1412,7 +1404,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1420,7 +1412,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1435,7 +1427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CA4446-BDCA-40AA-A549-CCDDEA333C10}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1443,13 +1435,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>25</v>
@@ -1458,13 +1450,13 @@
         <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
         <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -1514,7 +1506,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1591,28 +1583,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
       <c r="H1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
         <v>24</v>
@@ -1620,13 +1612,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2">
         <v>0.37</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -1634,13 +1626,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <v>250000</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -1648,13 +1640,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4">
         <v>800000</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4">
         <v>11</v>
@@ -1662,7 +1654,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="2">
         <v>2.5000000000000001E-2</v>
@@ -1670,7 +1662,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1697,7 +1689,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
@@ -1706,12 +1698,12 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1">
         <v>0.65</v>
@@ -1719,7 +1711,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4">
@@ -1729,7 +1721,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="5">
         <f>D4*C3*CapMarkets!B3</f>
@@ -1741,7 +1733,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="5">
         <f>SUM(C3:C4)</f>
@@ -1765,7 +1757,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -1774,12 +1766,12 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1787,7 +1779,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1">
         <v>0.6</v>
@@ -1795,7 +1787,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1803,7 +1795,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -1811,7 +1803,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2">
         <v>1.4999999999999999E-2</v>

</xml_diff>

<commit_message>
add fair value and permanent loan
</commit_message>
<xml_diff>
--- a/modera_decatur.xlsx
+++ b/modera_decatur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlp\Documents\GitHub\nus_apartment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA74538D-019F-467F-B4B7-FFA9CE3D0FCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066819EE-FDB7-480C-9E83-EF91888F1EC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="5205" windowWidth="16875" windowHeight="9195" firstSheet="6" activeTab="11" xr2:uid="{0613D09A-7280-4844-B453-E571AA672FAC}"/>
+    <workbookView xWindow="5625" yWindow="5205" windowWidth="16875" windowHeight="9195" firstSheet="6" activeTab="8" xr2:uid="{0613D09A-7280-4844-B453-E571AA672FAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Identification" sheetId="2" r:id="rId1"/>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771963C5-A621-408D-B251-D1D58ECD5746}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -976,7 +976,7 @@
         <v>38</v>
       </c>
       <c r="B2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
@@ -993,7 +993,7 @@
         <v>39</v>
       </c>
       <c r="B3">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -1010,8 +1010,8 @@
         <v>44</v>
       </c>
       <c r="B4">
-        <f>20*Identification!C11</f>
-        <v>4632980</v>
+        <f>8*Identification!C11</f>
+        <v>1853192</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
@@ -1749,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED12C745-5ACA-469A-A153-D935AE9EAECD}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1782,7 +1782,7 @@
         <v>63</v>
       </c>
       <c r="C3" s="1">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -1790,23 +1790,20 @@
         <v>64</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>66</v>
       </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="2">
-        <v>1.4999999999999999E-2</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>